<commit_message>
Updates template so that taxonomic coverage and total coverage are appended appropriately.
</commit_message>
<xml_diff>
--- a/data-raw/template/template.xlsx
+++ b/data-raw/template/template.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzyshaw/FlowWest/cvpiaEDIutils/data-raw/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE073D4-AC60-6140-A456-0E86AB03FB68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897FE817-FA27-1745-8775-536A619C6314}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16220" activeTab="2" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
+    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="16220" activeTab="1" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
     <sheet name="coverage" sheetId="2" r:id="rId2"/>
-    <sheet name="taxonomic coverage" sheetId="3" r:id="rId3"/>
+    <sheet name="taxonomic_coverage" sheetId="3" r:id="rId3"/>
+    <sheet name="nominal" sheetId="6" r:id="rId4"/>
+    <sheet name="ordinal" sheetId="7" r:id="rId5"/>
+    <sheet name="interval" sheetId="8" r:id="rId6"/>
+    <sheet name="ratio" sheetId="9" r:id="rId7"/>
+    <sheet name="dateTime" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="95">
   <si>
     <t>email</t>
   </si>
@@ -117,13 +122,208 @@
   </si>
   <si>
     <t>taxon_id</t>
+  </si>
+  <si>
+    <t>anamalia</t>
+  </si>
+  <si>
+    <t>chordata</t>
+  </si>
+  <si>
+    <t>mammalia</t>
+  </si>
+  <si>
+    <t>carnivora</t>
+  </si>
+  <si>
+    <t>felidae</t>
+  </si>
+  <si>
+    <t>panthera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">panthera leo </t>
+  </si>
+  <si>
+    <t>lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the first description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the second description </t>
+  </si>
+  <si>
+    <t>anamalias</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>taxonomic_coverage</t>
+  </si>
+  <si>
+    <t>steelhead</t>
+  </si>
+  <si>
+    <t>attribute_name</t>
+  </si>
+  <si>
+    <t>attribute_definition</t>
+  </si>
+  <si>
+    <t>storage_type</t>
+  </si>
+  <si>
+    <t>measurement_scale</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>text_pattern</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>attribute_label</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>unit_precision</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>number_type</t>
+  </si>
+  <si>
+    <t>date_time_format</t>
+  </si>
+  <si>
+    <t>date_time_precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is where it was </t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>the definition</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>this is where it is</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>this is the best attribute</t>
+  </si>
+  <si>
+    <t>an interval</t>
+  </si>
+  <si>
+    <t>the first interval</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>the second interval</t>
+  </si>
+  <si>
+    <t>a ratio</t>
+  </si>
+  <si>
+    <t>the first ratio</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>the second ratio</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">day </t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>gregorian</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>august</t>
+  </si>
+  <si>
+    <t>the month</t>
+  </si>
+  <si>
+    <t>add_taxonomic_coverage(CVPIA_common_species = "chinook")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +335,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,9 +368,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,7 +691,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>12345</v>
@@ -558,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40233F0A-2016-4048-9AE2-A8B67AED458C}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,9 +780,10 @@
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -594,6 +804,61 @@
       </c>
       <c r="G1" t="s">
         <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>-160.59399999999999</v>
+      </c>
+      <c r="C2">
+        <v>-134.10480000000001</v>
+      </c>
+      <c r="D2">
+        <v>71.238299999999995</v>
+      </c>
+      <c r="E2">
+        <v>67.864999999999995</v>
+      </c>
+      <c r="F2" s="2">
+        <v>29221</v>
+      </c>
+      <c r="G2" s="2">
+        <v>40543</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>-160.595</v>
+      </c>
+      <c r="C3">
+        <v>-134.10470000000001</v>
+      </c>
+      <c r="D3">
+        <v>71.238399999999999</v>
+      </c>
+      <c r="E3">
+        <v>67.866</v>
+      </c>
+      <c r="F3" s="2">
+        <v>29221</v>
+      </c>
+      <c r="G3" s="2">
+        <v>40543</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -603,10 +868,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5462ABFB-5B07-954F-BCDE-1E73F2959334}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,6 +914,644 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>183803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>183803</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C7E83F-9A95-794C-BFD5-AD3D50EF4E99}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE09427-81AB-1E41-887D-3E6C6FA5952B}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D9AEB2-91BD-A544-B597-8A642AAF92C8}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>100.111</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25F5318-96C9-6546-A09C-3A1112530D78}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>100</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F5B283-21E4-0C46-B1CE-3C517998F8DC}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates documentation for data table and attribute to be more thurough. Also adds all inputs to the template for easy use.
</commit_message>
<xml_diff>
--- a/data-raw/template/template.xlsx
+++ b/data-raw/template/template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzyshaw/FlowWest/cvpiaEDIutils/data-raw/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783B8FCE-9A74-F541-A65E-B1435983177B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B31C5F-1791-EB45-B456-BAD443994A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="900" windowWidth="27640" windowHeight="16220" activeTab="4" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
+    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="16220" activeTab="4" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
     <sheet name="coverage" sheetId="2" r:id="rId2"/>
     <sheet name="methods" sheetId="11" r:id="rId3"/>
     <sheet name="data_table" sheetId="14" r:id="rId4"/>
-    <sheet name="data table methods" sheetId="12" r:id="rId5"/>
+    <sheet name="data_table_methods" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>email</t>
   </si>
@@ -170,6 +170,21 @@
   </si>
   <si>
     <t xml:space="preserve">Not Applicable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">method 1 </t>
+  </si>
+  <si>
+    <t>this is the first method</t>
+  </si>
+  <si>
+    <t>ruler</t>
+  </si>
+  <si>
+    <t>method 2</t>
+  </si>
+  <si>
+    <t>this is the second method</t>
   </si>
 </sst>
 </file>
@@ -831,10 +846,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3274FFD5-571E-8948-86DE-91D5E0E7C9C1}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,6 +869,28 @@
         <v>30</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Includes a working xml template with all elements, as well as updated testing, documentation, and functions to fix the detected errors.
</commit_message>
<xml_diff>
--- a/data-raw/template/template.xlsx
+++ b/data-raw/template/template.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzyshaw/FlowWest/cvpiaEDIutils/data-raw/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B51C21D-B3DB-8144-95F6-9FB4F366C26D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A71C4BB-A66B-5644-B040-B49C3A0E8CE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="16220" activeTab="3" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
+    <workbookView xWindow="780" yWindow="880" windowWidth="27640" windowHeight="16220" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
     <sheet name="title" sheetId="15" r:id="rId2"/>
     <sheet name="license" sheetId="16" r:id="rId3"/>
-    <sheet name="keywordSet" sheetId="19" r:id="rId4"/>
-    <sheet name="funding" sheetId="17" r:id="rId5"/>
-    <sheet name="maintenance" sheetId="18" r:id="rId6"/>
-    <sheet name="coverage" sheetId="2" r:id="rId7"/>
-    <sheet name="methods" sheetId="11" r:id="rId8"/>
-    <sheet name="data_table" sheetId="14" r:id="rId9"/>
-    <sheet name="data_table_methods" sheetId="12" r:id="rId10"/>
+    <sheet name="keyword_set" sheetId="19" r:id="rId4"/>
+    <sheet name="attribute" sheetId="20" r:id="rId5"/>
+    <sheet name="funding" sheetId="17" r:id="rId6"/>
+    <sheet name="maintenance" sheetId="18" r:id="rId7"/>
+    <sheet name="taxonomic_coverage" sheetId="21" r:id="rId8"/>
+    <sheet name="code_definitions" sheetId="24" r:id="rId9"/>
+    <sheet name="physical" sheetId="22" r:id="rId10"/>
+    <sheet name="coverage" sheetId="2" r:id="rId11"/>
+    <sheet name="methods" sheetId="11" r:id="rId12"/>
+    <sheet name="data_table" sheetId="14" r:id="rId13"/>
+    <sheet name="data_table_methods" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
   <si>
     <t>email</t>
   </si>
@@ -63,9 +67,6 @@
     <t>jdoe@gmail.com</t>
   </si>
   <si>
-    <t>creator</t>
-  </si>
-  <si>
     <t>FlowWest</t>
   </si>
   <si>
@@ -120,36 +121,15 @@
     <t>add_taxonomic_coverage(CVPIA_common_species = "chinook")</t>
   </si>
   <si>
-    <t xml:space="preserve">title </t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>instrumentation</t>
   </si>
   <si>
     <t>title</t>
   </si>
   <si>
-    <t>method 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is the first method we used </t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
-    <t xml:space="preserve">method 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is the second method we used </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ruler </t>
-  </si>
-  <si>
     <t>entity_name</t>
   </si>
   <si>
@@ -177,21 +157,9 @@
     <t xml:space="preserve">Not Applicable </t>
   </si>
   <si>
-    <t xml:space="preserve">method 1 </t>
-  </si>
-  <si>
-    <t>this is the first method</t>
-  </si>
-  <si>
     <t>ruler</t>
   </si>
   <si>
-    <t>method 2</t>
-  </si>
-  <si>
-    <t>this is the second method</t>
-  </si>
-  <si>
     <t>short_name</t>
   </si>
   <si>
@@ -240,9 +208,6 @@
     <t xml:space="preserve">status </t>
   </si>
   <si>
-    <t>update_frequeny</t>
-  </si>
-  <si>
     <t xml:space="preserve">ongoing </t>
   </si>
   <si>
@@ -252,9 +217,6 @@
     <t>keyword</t>
   </si>
   <si>
-    <t>keywordThesauraus</t>
-  </si>
-  <si>
     <t>chinook</t>
   </si>
   <si>
@@ -268,6 +230,225 @@
   </si>
   <si>
     <t>LTER controlled vocabulary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attribute_name </t>
+  </si>
+  <si>
+    <t>attribute_definition</t>
+  </si>
+  <si>
+    <t>storage_type</t>
+  </si>
+  <si>
+    <t>measurement_scale</t>
+  </si>
+  <si>
+    <t>keywordThesaurus</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>phylum</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">species </t>
+  </si>
+  <si>
+    <t xml:space="preserve">common_name </t>
+  </si>
+  <si>
+    <t>taxon_id</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>attribute_label</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>text_pattern</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>number_type</t>
+  </si>
+  <si>
+    <t>unit_precision</t>
+  </si>
+  <si>
+    <t>date_time_format</t>
+  </si>
+  <si>
+    <t>date_time_precision</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">methods_file </t>
+  </si>
+  <si>
+    <t>inst/extdata/methods-template.docx</t>
+  </si>
+  <si>
+    <t>inst/extdata/abstract_template.docx</t>
+  </si>
+  <si>
+    <t>file_path</t>
+  </si>
+  <si>
+    <t>number_of_headers</t>
+  </si>
+  <si>
+    <t>record_delimiter</t>
+  </si>
+  <si>
+    <t>attribute_orientation</t>
+  </si>
+  <si>
+    <t>field_delimiter</t>
+  </si>
+  <si>
+    <t>data_url</t>
+  </si>
+  <si>
+    <t>/Users/lizzyshaw/FlowWest/cvpiaEDIutils/tests/testthat/test_data.csv</t>
+  </si>
+  <si>
+    <t>mydata.org</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>CVPIA_common_species</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definitions</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>horse</t>
+  </si>
+  <si>
+    <t>monkey</t>
+  </si>
+  <si>
+    <t>pet</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>wild</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>this is a dog</t>
+  </si>
+  <si>
+    <t>this is a cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">whole </t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>to the year</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
+  </si>
+  <si>
+    <t>identity</t>
+  </si>
+  <si>
+    <t>funding</t>
+  </si>
+  <si>
+    <t>myfunding.org</t>
+  </si>
+  <si>
+    <t>provides funding for cvpia project</t>
+  </si>
+  <si>
+    <t>update_frequency</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-4151-6081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data manager </t>
   </si>
 </sst>
 </file>
@@ -312,13 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -639,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE1A70B-0713-AF47-A707-CB0A71DE9B9F}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,89 +854,364 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2">
-        <v>12345</v>
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3">
-        <v>6789</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{3AE588B5-A088-3345-8669-FE1C3D856B75}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F9D885D1-5A53-3A4B-86A4-F75F01B6EA9D}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{A670B382-8DCD-854A-8BFE-3C3B1067DC94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3274FFD5-571E-8948-86DE-91D5E0E7C9C1}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85692C7A-614D-114E-BBDD-87F6D172CE74}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="1" max="1" width="61.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40233F0A-2016-4048-9AE2-A8B67AED458C}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>-160.59399999999999</v>
+      </c>
+      <c r="C2">
+        <v>-134.10480000000001</v>
+      </c>
+      <c r="D2">
+        <v>71.238299999999995</v>
+      </c>
+      <c r="E2">
+        <v>67.864999999999995</v>
+      </c>
+      <c r="F2" s="2">
+        <v>29221</v>
+      </c>
+      <c r="G2" s="2">
+        <v>40543</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>-160.595</v>
+      </c>
+      <c r="C3">
+        <v>-134.10470000000001</v>
+      </c>
+      <c r="D3">
+        <v>71.238399999999999</v>
+      </c>
+      <c r="E3">
+        <v>67.866</v>
+      </c>
+      <c r="F3" s="2">
+        <v>29221</v>
+      </c>
+      <c r="G3" s="2">
+        <v>40543</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203B1F42-BC15-F74A-922C-2D796F75006E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6C103A-5382-7E43-937F-29C0659651C2}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3274FFD5-571E-8948-86DE-91D5E0E7C9C1}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -782,18 +1235,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>53</v>
+      <c r="A2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -819,24 +1272,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -848,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DF32E5-7427-724F-B57A-9FA2CFD4337E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,42 +1313,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -904,11 +1357,209 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3816F74F-2852-5147-8D34-33C645A313FC}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07891161-E000-BC46-A3D6-753B870581A9}">
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4">
+        <v>1E-3</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3816F74F-2852-5147-8D34-33C645A313FC}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,22 +1572,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>123456</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -944,12 +1615,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4052469-3958-8744-9545-65D024A843E0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,119 +1630,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40233F0A-2016-4048-9AE2-A8B67AED458C}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" customWidth="1"/>
-    <col min="8" max="8" width="53.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>-160.59399999999999</v>
-      </c>
-      <c r="C2">
-        <v>-134.10480000000001</v>
-      </c>
-      <c r="D2">
-        <v>71.238299999999995</v>
-      </c>
-      <c r="E2">
-        <v>67.864999999999995</v>
-      </c>
-      <c r="F2" s="2">
-        <v>29221</v>
-      </c>
-      <c r="G2" s="2">
-        <v>40543</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>-160.595</v>
-      </c>
-      <c r="C3">
-        <v>-134.10470000000001</v>
-      </c>
-      <c r="D3">
-        <v>71.238399999999999</v>
-      </c>
-      <c r="E3">
-        <v>67.866</v>
-      </c>
-      <c r="F3" s="2">
-        <v>29221</v>
-      </c>
-      <c r="G3" s="2">
-        <v>40543</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1080,50 +1650,58 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{203B1F42-BC15-F74A-922C-2D796F75006E}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5797B12-C25B-2440-BF9A-9513196783AA}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1132,61 +1710,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6C103A-5382-7E43-937F-29C0659651C2}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A322816C-3F87-0F4A-BC97-A8FBB208641A}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds a csv file for the physical example and also updates the template with further Hannon data.
</commit_message>
<xml_diff>
--- a/data-raw/template/template.xlsx
+++ b/data-raw/template/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzyshaw/FlowWest/cvpiaEDIutils/data-raw/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0887E8C2-A1F0-0D44-84F8-923DBAF5C040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A428F872-74AB-DD4B-8FA0-6FBC3C55E188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16220" firstSheet="3" activeTab="13" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
+    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16220" firstSheet="3" activeTab="11" xr2:uid="{37ED225B-808D-884D-A6F1-049399879715}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
   <si>
     <t>email</t>
   </si>
@@ -86,9 +86,6 @@
     <t>steelhead</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>instrumentation</t>
   </si>
   <si>
@@ -239,18 +236,6 @@
     <t>nominal</t>
   </si>
   <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>ordinal</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>cool</t>
-  </si>
-  <si>
     <t xml:space="preserve">methods_file </t>
   </si>
   <si>
@@ -269,63 +254,15 @@
     <t>definitions</t>
   </si>
   <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>horse</t>
-  </si>
-  <si>
-    <t>monkey</t>
-  </si>
-  <si>
-    <t>pet</t>
-  </si>
-  <si>
-    <t>farm</t>
-  </si>
-  <si>
-    <t>wild</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
-    <t>interval</t>
-  </si>
-  <si>
     <t>dateTime</t>
   </si>
   <si>
-    <t xml:space="preserve">no label </t>
-  </si>
-  <si>
-    <t xml:space="preserve">whole </t>
-  </si>
-  <si>
-    <t>years</t>
-  </si>
-  <si>
-    <t>to the year</t>
-  </si>
-  <si>
     <t>update_frequency</t>
   </si>
   <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>third</t>
-  </si>
-  <si>
     <t>Hannon</t>
   </si>
   <si>
@@ -404,9 +341,6 @@
     <t>ongoing</t>
   </si>
   <si>
-    <t>data-raw/Hannon-Example/hannon_example_physical_data.xlsx</t>
-  </si>
-  <si>
     <t>Variables</t>
   </si>
   <si>
@@ -419,13 +353,52 @@
     <t>data-raw/Hannon-Example/hannon_example_abstract.docx</t>
   </si>
   <si>
-    <t>fourth</t>
-  </si>
-  <si>
     <t>attribute_name</t>
   </si>
   <si>
     <t>enumerated</t>
+  </si>
+  <si>
+    <t>data-raw/Hannon-Example/hannon_example_physical_data.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The weather on that day </t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Partly Cloudy</t>
+  </si>
+  <si>
+    <t>Cloudy</t>
+  </si>
+  <si>
+    <t>Rain</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fog </t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The day tha the data was collected </t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>YYYY '-' MM '-' DD</t>
   </si>
 </sst>
 </file>
@@ -489,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -506,6 +479,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -856,63 +830,63 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -938,39 +912,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -988,7 +962,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,15 +972,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1016,189 +990,124 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07891161-E000-BC46-A3D6-753B870581A9}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="9" max="9" width="5.5" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" customWidth="1"/>
-    <col min="15" max="15" width="8.83203125" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4">
-        <v>1E-3</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" t="s">
-        <v>88</v>
-      </c>
-      <c r="N5" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
+      <c r="F2" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="5">
+        <v>42346</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1211,86 +1120,89 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3274FFD5-571E-8948-86DE-91D5E0E7C9C1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1314,15 +1226,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1348,24 +1260,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,18 +1304,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1427,25 +1339,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1468,12 +1380,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1499,24 +1411,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1543,36 +1455,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C2" s="3">
         <v>12345</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1597,18 +1509,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1633,15 +1545,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1692,7 +1604,7 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B2" s="3">
         <v>-122.448217</v>
@@ -1710,7 +1622,7 @@
         <v>42370</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>